<commit_message>
Stephen's additions to proposal
</commit_message>
<xml_diff>
--- a/PastProjectAnalysis.xlsx
+++ b/PastProjectAnalysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taniy\Desktop\Spring18\6301.502\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="6450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="old proejcts analysis" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="143">
   <si>
     <t>Semester</t>
   </si>
@@ -367,13 +367,107 @@
   </si>
   <si>
     <t xml:space="preserve">Mininet, controller Ryu, pfSense firewall </t>
+  </si>
+  <si>
+    <t>https://www.parrotsec.org/</t>
+  </si>
+  <si>
+    <t>Parrot Security OS for Security Testing</t>
+  </si>
+  <si>
+    <t>https://metasploit.help.rapid7.com/docs/metasploitable-2-exploitability-guide</t>
+  </si>
+  <si>
+    <t>Metasploitable 2 - For generating attacks</t>
+  </si>
+  <si>
+    <t>Snort IDS</t>
+  </si>
+  <si>
+    <t>https://www.snort.org/</t>
+  </si>
+  <si>
+    <t>Datasets for ML for various types of attacks</t>
+  </si>
+  <si>
+    <t>http://www.unb.ca/cic/datasets/index.html</t>
+  </si>
+  <si>
+    <t>NSL-KDD Dataset used in above paper</t>
+  </si>
+  <si>
+    <t>http://www.unb.ca/cic/datasets/nsl.html</t>
+  </si>
+  <si>
+    <t>Most recent dataset</t>
+  </si>
+  <si>
+    <t>http://www.unb.ca/cic/datasets/ids-2017.html</t>
+  </si>
+  <si>
+    <t>Intrusion Detection dataset</t>
+  </si>
+  <si>
+    <t>http://www.unb.ca/cic/datasets/ids.html</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Adaboost</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Naïve Bayes</t>
+  </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>Self-Organizing Maps</t>
+  </si>
+  <si>
+    <t>Stephen Thoughts</t>
+  </si>
+  <si>
+    <t>Too generic.  The functionalities listed cover most of the range of all the previous projects combined.
+1) Test all controllers
+2) IDS/Firewall
+3) QoS/Bandwidth Management
+One or two of those may be difficult.  Doing all 3 in a few months may not be viable.</t>
+  </si>
+  <si>
+    <t>ML portion can be a "stretch goal" - if we are able to achieve the other parts of our project, then we can work on this.
+From ML-perspective, I was able to find datasets for IDS and other security-related issues.  I also found the tools we can use to generate the security issues we want to watch for.
+QoS and bandwidth are harder for ML, because I couldn't easily find datasets for those.  We would also probably have to generate our own traffic (Skype, etc?).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think doing both IDS and QoS may be too large of a project.  </t>
+  </si>
+  <si>
+    <t>To implement and compare various open source controllers available. We will set up networks using each controller (Ryu, Open Daylight, ONOS, POX, Floodlight) and test firewall and intrusion detection on each controller. We plan to use pfSense as our firewall, Snort as an IDS, and various tools to generate intrusions and attacks.
+As a stretch-goal (i.e. able to complete everything mentioned above), we will use Machine Learning to design an application that is able to detect intrusions and detect unwanted traffic on the network.</t>
+  </si>
+  <si>
+    <t>Mininet, controllers (Ryu, Open Daylight, ONOS, POX, Floodlight), pfSense (firewall), Snort (IDS)</t>
+  </si>
+  <si>
+    <t>Tools Used from Paper: "ML-Based IDS for SDN"</t>
+  </si>
+  <si>
+    <t>ML Techniques Used in papers</t>
+  </si>
+  <si>
+    <t>&lt;---- Stephen's Proposal based on the above proposals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,8 +491,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,8 +520,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -441,26 +556,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -491,7 +762,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -803,21 +1074,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -834,7 +1105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -848,7 +1119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -865,7 +1136,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -879,7 +1150,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -896,7 +1167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -907,7 +1178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -921,7 +1192,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -935,7 +1206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -952,7 +1223,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -969,7 +1240,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -980,7 +1251,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -988,7 +1259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -999,7 +1270,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1013,7 +1284,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1027,7 +1298,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1038,7 +1309,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1049,7 +1320,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1057,7 +1328,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1065,7 +1336,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1076,7 +1347,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1084,7 +1355,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1092,7 +1363,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1100,7 +1371,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1111,7 +1382,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1119,7 +1390,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1130,7 +1401,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1138,7 +1409,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1146,7 +1417,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1154,7 +1425,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -1162,7 +1433,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1173,7 +1444,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1181,7 +1452,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -1192,7 +1463,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1200,7 +1471,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -1211,7 +1482,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -1222,7 +1493,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -1233,7 +1504,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -1241,7 +1512,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -1249,7 +1520,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1260,7 +1531,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -1268,7 +1539,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -1276,7 +1547,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -1284,7 +1555,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -1292,7 +1563,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -1300,7 +1571,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -1308,7 +1579,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -1316,7 +1587,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -1330,7 +1601,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -1344,7 +1615,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -1358,7 +1629,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -1372,7 +1643,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -1386,7 +1657,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -1400,7 +1671,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -1414,7 +1685,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -1428,7 +1699,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -1442,7 +1713,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -1456,7 +1727,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -1470,7 +1741,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>88</v>
       </c>
@@ -1486,75 +1757,229 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1"/>
-    <hyperlink ref="E50" r:id="rId2"/>
-    <hyperlink ref="E49" r:id="rId3"/>
-    <hyperlink ref="E51" r:id="rId4"/>
-    <hyperlink ref="E52" r:id="rId5"/>
-    <hyperlink ref="E53" r:id="rId6"/>
-    <hyperlink ref="E54" r:id="rId7"/>
-    <hyperlink ref="E55" r:id="rId8"/>
-    <hyperlink ref="E56" r:id="rId9"/>
-    <hyperlink ref="E57" r:id="rId10"/>
-    <hyperlink ref="E58" r:id="rId11"/>
-    <hyperlink ref="E59" r:id="rId12"/>
-    <hyperlink ref="E60" r:id="rId13"/>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E50" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E49" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E51" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E52" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E53" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E54" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E55" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E56" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E57" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E58" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E59" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E60" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="137.109375" customWidth="1"/>
-    <col min="2" max="2" width="35.5546875" customWidth="1"/>
+    <col min="1" max="1" width="137.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="74.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>112</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="C3" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="26"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="26"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B22:C25"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{8AFC4C8B-DA41-4A1D-91CE-499C29E07138}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{B5CCF6B4-AF4C-4288-83C8-33DCD5487DD0}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{AE25DA5F-3930-455A-BFFB-B6DC3E5A575F}"/>
+    <hyperlink ref="B12" r:id="rId4" xr:uid="{39D0E9E8-C8AF-4438-BC00-780BDF961918}"/>
+    <hyperlink ref="B13" r:id="rId5" xr:uid="{8C2673AD-77B6-453C-BF9C-79A652E45259}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{D8CE5E34-F4D5-4F40-B204-AA2B0089F424}"/>
+    <hyperlink ref="B15" r:id="rId7" xr:uid="{9E7FD5B1-9ABE-4399-AC34-1A881961E81B}"/>
+    <hyperlink ref="B16" r:id="rId8" xr:uid="{AA125322-5BE9-4742-9D20-2688E65856DE}"/>
+    <hyperlink ref="B22" r:id="rId9" xr:uid="{E079DD83-D43E-4C4F-BFCA-77BB2A7D1D72}"/>
+    <hyperlink ref="B26" r:id="rId10" xr:uid="{7E4F614C-6BA3-432D-B690-66D3C38BD8E8}"/>
+    <hyperlink ref="B27" r:id="rId11" xr:uid="{B195646D-4C90-4827-AEE7-892A26E6B67B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>